<commit_message>
Question Bank Last upload
</commit_message>
<xml_diff>
--- a/Question Bank.xlsx
+++ b/Question Bank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Question Bank" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t xml:space="preserve">S. No.</t>
   </si>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">All of above</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 13</t>
+    <t xml:space="preserve">Option – 1</t>
   </si>
   <si>
     <t xml:space="preserve">How to get all keys from a dictionary?</t>
@@ -229,9 +229,6 @@
     <t xml:space="preserve">let allKeys = Array(myKey.keys)</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 14</t>
-  </si>
-  <si>
     <t xml:space="preserve">How to get all values from a dictionary?</t>
   </si>
   <si>
@@ -241,7 +238,7 @@
     <t xml:space="preserve">let allValues = Array(myValue.values)</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 15</t>
+    <t xml:space="preserve">Option – 12</t>
   </si>
   <si>
     <t xml:space="preserve">Is it possible to append an array with another array?</t>
@@ -259,15 +256,9 @@
     <t xml:space="preserve">Never</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 16</t>
-  </si>
-  <si>
     <t xml:space="preserve">Is it possible to check if object is a dictionary?</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 17</t>
-  </si>
-  <si>
     <t xml:space="preserve">“dict1.isEmpty” is the return type of?</t>
   </si>
   <si>
@@ -280,9 +271,6 @@
     <t xml:space="preserve">String</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Which protocol does dictionary conform to?</t>
   </si>
   <si>
@@ -298,16 +286,10 @@
     <t xml:space="preserve">Hashable</t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 19</t>
-  </si>
-  <si>
     <t xml:space="preserve">let dictionary1 [String: [String]] = [:[]] -is this a valid declaration? </t>
   </si>
   <si>
-    <t xml:space="preserve">Option – 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option – 21</t>
+    <t xml:space="preserve">Option – </t>
   </si>
 </sst>
 </file>
@@ -317,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -362,12 +344,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -425,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,14 +432,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -550,20 +518,20 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topRight" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.1214574898785"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1457489878543"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2672064777328"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -684,7 +652,7 @@
       <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -702,13 +670,13 @@
       <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -750,7 +718,7 @@
       <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -880,7 +848,7 @@
         <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="H13" s="7"/>
     </row>
@@ -888,14 +856,14 @@
       <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
@@ -904,7 +872,7 @@
         <v>54</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="7"/>
     </row>
@@ -913,22 +881,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="G15" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -937,22 +905,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="H16" s="7"/>
     </row>
@@ -961,22 +929,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="H17" s="7"/>
     </row>
@@ -985,22 +953,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -1009,22 +977,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="G19" s="4" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -1038,7 +1006,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H20" s="7"/>
     </row>

</xml_diff>